<commit_message>
Files reorganized. Merging datasets figured out
</commit_message>
<xml_diff>
--- a/other_data/chronology.xlsx
+++ b/other_data/chronology.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>05-03-2020</t>
   </si>
@@ -123,13 +123,16 @@
     <t>мэр подписал указ о выплатах донорам плазмы крови с антителами на коронавирус. Донорами могут стать лица, которые переболели коронавирусной инфекцией и выработали иммунитет, не имеют хронических заболеваний и противопоказаний. Выплаты составляют 1250 руб. за каждые 150 мл плазмы. Минимальный объём сдачи — 300 мл, максимальный — 600 мл</t>
   </si>
   <si>
-    <t>Published</t>
-  </si>
-  <si>
     <t>Descriprion</t>
   </si>
   <si>
     <t>Власти Москвы временно отменили бесплатный проезд в транспорте для студентов и пожилых людей старше 65 лет. Кроме того, с 26 марта по 14 апреля был введён режим самоизоляции для лиц старше 65 лет и тех, кто страдает хроническими заболеваниями.Указом от 25.03.2020  №206 Президент РФ  Путин В.В. объявил нерабочими днями  период с 30.03.2020 г. по 03.04.2020 г.</t>
+  </si>
+  <si>
+    <t>step_number</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -463,9 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -477,10 +478,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
+      <c r="C1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -490,6 +494,9 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -501,6 +508,9 @@
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -512,6 +522,9 @@
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -520,13 +533,19 @@
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -536,6 +555,9 @@
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="174" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -544,6 +566,9 @@
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -552,6 +577,9 @@
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -560,6 +588,9 @@
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -568,6 +599,9 @@
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -576,6 +610,9 @@
       <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
@@ -584,6 +621,9 @@
       <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
@@ -592,6 +632,9 @@
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
@@ -600,6 +643,9 @@
       <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
@@ -608,64 +654,70 @@
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="5"/>
     </row>

</xml_diff>